<commit_message>
Update asset 3D models and wiring
</commit_message>
<xml_diff>
--- a/assets/ESP32_Wiring.xlsx
+++ b/assets/ESP32_Wiring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ahmoa-my.sharepoint.com/personal/francois_boldoduck_ahmoa_fr/Documents/!!! Robotique !!!/SW_MSE-6/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{E204F435-9A13-49BB-A2EE-85C1E68357FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE9B2DB6-9C74-4C7B-B23B-5DE47A2D1007}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="8_{E204F435-9A13-49BB-A2EE-85C1E68357FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB91A76E-2F36-4F32-AA5E-E721B20DD20F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{03262896-5594-4AD1-BF64-377D9006D926}"/>
+    <workbookView xWindow="28680" yWindow="-2010" windowWidth="16440" windowHeight="28320" xr2:uid="{03262896-5594-4AD1-BF64-377D9006D926}"/>
   </bookViews>
   <sheets>
     <sheet name="ESP32" sheetId="1" r:id="rId1"/>
@@ -292,7 +292,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -332,6 +332,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -348,7 +354,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -357,6 +363,7 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Insatisfaisant" xfId="2" builtinId="27"/>
@@ -384,13 +391,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>211844</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>16932</xdr:rowOff>
+      <xdr:rowOff>48682</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>72157</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>33499</xdr:rowOff>
+      <xdr:rowOff>65249</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -418,8 +425,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4335111" y="203199"/>
-          <a:ext cx="11002446" cy="6349633"/>
+          <a:off x="4180594" y="239182"/>
+          <a:ext cx="10528313" cy="6493567"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -438,7 +445,142 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>179293</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>100854</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>159774</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>134470</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{311919BF-5E55-5D77-1998-865FF80DF3EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect b="57812"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4146175" y="6958854"/>
+          <a:ext cx="6076481" cy="3653116"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>179293</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>740751</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>141719</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6523FD9F-4777-CE9D-8CD5-92F48D65C8D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10298206" y="7037293"/>
+          <a:ext cx="4315427" cy="3772426"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>123264</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>123264</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>6603</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D2AC2A2-B582-64FC-A6A6-10A5D1564EB0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="123264" y="8124264"/>
+          <a:ext cx="3850221" cy="2207559"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -740,16 +882,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED68F266-D7F2-40F4-B71A-211722391F5C}">
   <dimension ref="B2:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="90" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>43</v>
       </c>
@@ -757,7 +899,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -765,13 +907,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>2</v>
       </c>
@@ -779,7 +921,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>3</v>
       </c>
@@ -787,7 +929,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>4</v>
       </c>
@@ -795,7 +937,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>5</v>
       </c>
@@ -803,7 +945,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>6</v>
       </c>
@@ -811,7 +953,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>7</v>
       </c>
@@ -819,7 +961,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>8</v>
       </c>
@@ -827,7 +969,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>9</v>
       </c>
@@ -835,7 +977,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>10</v>
       </c>
@@ -843,7 +985,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>11</v>
       </c>
@@ -851,13 +993,13 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>13</v>
       </c>
@@ -865,13 +1007,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>15</v>
       </c>
@@ -879,7 +1021,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>16</v>
       </c>
@@ -887,7 +1029,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>17</v>
       </c>
@@ -895,7 +1037,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>18</v>
       </c>
@@ -903,43 +1045,43 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>19</v>
       </c>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>21</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D25" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>24</v>
       </c>
@@ -947,7 +1089,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>25</v>
       </c>
@@ -955,7 +1097,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>26</v>
       </c>
@@ -963,31 +1105,31 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>31</v>
       </c>
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>32</v>
       </c>
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>33</v>
       </c>
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>34</v>
       </c>
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>35</v>
       </c>
@@ -995,16 +1137,16 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
+      <c r="D35" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="8" t="s">
         <v>61</v>
       </c>
       <c r="C36" t="s">
@@ -1014,8 +1156,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="8" t="s">
         <v>61</v>
       </c>
       <c r="C37" t="s">
@@ -1025,8 +1167,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="s">
         <v>61</v>
       </c>
       <c r="C38" t="s">
@@ -1034,20 +1176,20 @@
       </c>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>40</v>
       </c>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>41</v>
       </c>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="8" t="s">
         <v>61</v>
       </c>
       <c r="C41" t="s">

</xml_diff>